<commit_message>
codes color & internal note
</commit_message>
<xml_diff>
--- a/app/static/uploads/pkn_old_codes.xlsx
+++ b/app/static/uploads/pkn_old_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dp/PKN/app/static/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B896FCAC-73D4-C249-A070-4EF949E068BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2751D2B1-A4AB-4047-8C96-A03BE2437044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="820" windowWidth="47600" windowHeight="25400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14196,9 +14196,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY1399"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>